<commit_message>
Added links to Bill of Material
</commit_message>
<xml_diff>
--- a/Documentation/Assembly Instructions/Bill of Materials-gliax_ecg_simple-simplified_format.xlsx
+++ b/Documentation/Assembly Instructions/Bill of Materials-gliax_ecg_simple-simplified_format.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/jgivans_uwo_ca/Documents/Glia/jg_version/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/jgivans_uwo_ca/Documents/Glia/RepoFork/ecg/Documentation/Assembly Instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCFE0F16-777C-4DBE-AA7C-797BB91726B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{FCFE0F16-777C-4DBE-AA7C-797BB91726B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA37CA89-77C7-4976-9F11-D8BF316BEBC5}"/>
   <bookViews>
-    <workbookView xWindow="-16590" yWindow="9225" windowWidth="34650" windowHeight="17565" xr2:uid="{EEB06583-8D90-45EE-9B4C-5B55527DF81E}"/>
+    <workbookView xWindow="13455" yWindow="2970" windowWidth="25785" windowHeight="16350" xr2:uid="{EEB06583-8D90-45EE-9B4C-5B55527DF81E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bill of Materials-gliax_ecg_sim" sheetId="1" r:id="rId1"/>
+    <sheet name="Bill of Materials-gliax_ecg" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-gliax_ecg_sim'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-gliax_ecg'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1229,10 +1229,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2BCDBA-DD07-45C9-BA56-6AF9FBBFED5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A9D4A4-3BDB-43BB-AA76-D881B793937A}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>

</xml_diff>